<commit_message>
New TMT with more images
</commit_message>
<xml_diff>
--- a/TMT_fmri/Only_TMTA_TMTA.xlsx
+++ b/TMT_fmri/Only_TMTA_TMTA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunduniversityo365-my.sharepoint.com/personal/pi6342kl_lu_se/Documents/Biofinder/fMRI-tasks/TrailMakingTask_fMRI/TMT_fmri/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_F25DC773A252ABDACC1048BC415F7C7A5ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69D1F1AE-4681-4137-B63E-CC0E1524CCE8}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_F25DC773A252ABDACC1048BC415F7C7A5ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{322E3518-5236-432A-B39C-A5AA6460D754}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="3675" windowWidth="21585" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5010" yWindow="2610" windowWidth="21585" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7707,12 +7707,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G834"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A809" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A834" sqref="A834:XFD834"/>
+    <sheetView tabSelected="1" topLeftCell="A714" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A809" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="4" max="4" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.7109375" bestFit="1" customWidth="1"/>
@@ -7720,7 +7721,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1992</v>
       </c>
       <c r="B1" t="s">
@@ -8343,7 +8344,6 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
@@ -8960,7 +8960,6 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
@@ -9577,7 +9576,6 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
@@ -10194,7 +10192,6 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
@@ -10811,7 +10808,6 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
@@ -11428,7 +11424,6 @@
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
@@ -12045,7 +12040,6 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1" t="s">
@@ -12662,7 +12656,6 @@
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1" t="s">
@@ -12679,7 +12672,7 @@
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A210">
+      <c r="A210" s="1">
         <v>1</v>
       </c>
       <c r="B210" t="s">
@@ -12702,7 +12695,7 @@
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A211">
+      <c r="A211" s="1">
         <v>2</v>
       </c>
       <c r="B211" t="s">
@@ -12725,7 +12718,7 @@
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A212">
+      <c r="A212" s="1">
         <v>3</v>
       </c>
       <c r="B212" t="s">
@@ -12748,7 +12741,7 @@
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A213">
+      <c r="A213" s="1">
         <v>4</v>
       </c>
       <c r="B213" t="s">
@@ -12771,7 +12764,7 @@
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A214">
+      <c r="A214" s="1">
         <v>5</v>
       </c>
       <c r="B214" t="s">
@@ -12794,7 +12787,7 @@
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A215">
+      <c r="A215" s="1">
         <v>6</v>
       </c>
       <c r="B215" t="s">
@@ -12817,7 +12810,7 @@
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A216">
+      <c r="A216" s="1">
         <v>7</v>
       </c>
       <c r="B216" t="s">
@@ -12840,7 +12833,7 @@
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A217">
+      <c r="A217" s="1">
         <v>8</v>
       </c>
       <c r="B217" t="s">
@@ -12863,7 +12856,7 @@
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A218">
+      <c r="A218" s="1">
         <v>9</v>
       </c>
       <c r="B218" t="s">
@@ -12886,7 +12879,7 @@
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A219">
+      <c r="A219" s="1">
         <v>10</v>
       </c>
       <c r="B219" t="s">
@@ -12909,7 +12902,7 @@
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A220">
+      <c r="A220" s="1">
         <v>11</v>
       </c>
       <c r="B220" t="s">
@@ -12932,7 +12925,7 @@
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A221">
+      <c r="A221" s="1">
         <v>12</v>
       </c>
       <c r="B221" t="s">
@@ -12955,7 +12948,7 @@
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A222">
+      <c r="A222" s="1">
         <v>13</v>
       </c>
       <c r="B222" t="s">
@@ -12978,7 +12971,7 @@
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A223">
+      <c r="A223" s="1">
         <v>14</v>
       </c>
       <c r="B223" t="s">
@@ -13001,7 +12994,7 @@
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A224">
+      <c r="A224" s="1">
         <v>15</v>
       </c>
       <c r="B224" t="s">
@@ -13024,7 +13017,7 @@
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A225">
+      <c r="A225" s="1">
         <v>16</v>
       </c>
       <c r="B225" t="s">
@@ -13047,7 +13040,7 @@
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A226">
+      <c r="A226" s="1">
         <v>17</v>
       </c>
       <c r="B226" t="s">
@@ -13070,7 +13063,7 @@
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A227">
+      <c r="A227" s="1">
         <v>18</v>
       </c>
       <c r="B227" t="s">
@@ -13093,7 +13086,7 @@
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A228">
+      <c r="A228" s="1">
         <v>19</v>
       </c>
       <c r="B228" t="s">
@@ -13116,7 +13109,7 @@
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A229">
+      <c r="A229" s="1">
         <v>20</v>
       </c>
       <c r="B229" t="s">
@@ -13139,7 +13132,7 @@
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A230">
+      <c r="A230" s="1">
         <v>21</v>
       </c>
       <c r="B230" t="s">
@@ -13162,7 +13155,7 @@
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A231">
+      <c r="A231" s="1">
         <v>22</v>
       </c>
       <c r="B231" t="s">
@@ -13185,7 +13178,7 @@
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A232">
+      <c r="A232" s="1">
         <v>23</v>
       </c>
       <c r="B232" t="s">
@@ -13208,7 +13201,7 @@
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A233">
+      <c r="A233" s="1">
         <v>24</v>
       </c>
       <c r="B233" t="s">
@@ -13231,7 +13224,7 @@
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A234">
+      <c r="A234" s="1">
         <v>25</v>
       </c>
       <c r="B234" t="s">
@@ -13268,7 +13261,7 @@
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A236">
+      <c r="A236" s="1">
         <v>1</v>
       </c>
       <c r="B236" t="s">
@@ -13291,7 +13284,7 @@
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A237">
+      <c r="A237" s="1">
         <v>2</v>
       </c>
       <c r="B237" t="s">
@@ -13314,7 +13307,7 @@
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A238">
+      <c r="A238" s="1">
         <v>3</v>
       </c>
       <c r="B238" t="s">
@@ -13337,7 +13330,7 @@
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A239">
+      <c r="A239" s="1">
         <v>4</v>
       </c>
       <c r="B239" t="s">
@@ -13360,7 +13353,7 @@
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A240">
+      <c r="A240" s="1">
         <v>5</v>
       </c>
       <c r="B240" t="s">
@@ -13383,7 +13376,7 @@
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A241">
+      <c r="A241" s="1">
         <v>6</v>
       </c>
       <c r="B241" t="s">
@@ -13406,7 +13399,7 @@
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A242">
+      <c r="A242" s="1">
         <v>7</v>
       </c>
       <c r="B242" t="s">
@@ -13429,7 +13422,7 @@
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A243">
+      <c r="A243" s="1">
         <v>8</v>
       </c>
       <c r="B243" t="s">
@@ -13452,7 +13445,7 @@
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244">
+      <c r="A244" s="1">
         <v>9</v>
       </c>
       <c r="B244" t="s">
@@ -13475,7 +13468,7 @@
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A245">
+      <c r="A245" s="1">
         <v>10</v>
       </c>
       <c r="B245" t="s">
@@ -13498,7 +13491,7 @@
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A246">
+      <c r="A246" s="1">
         <v>11</v>
       </c>
       <c r="B246" t="s">
@@ -13521,7 +13514,7 @@
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A247">
+      <c r="A247" s="1">
         <v>12</v>
       </c>
       <c r="B247" t="s">
@@ -13544,7 +13537,7 @@
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A248">
+      <c r="A248" s="1">
         <v>13</v>
       </c>
       <c r="B248" t="s">
@@ -13567,7 +13560,7 @@
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A249">
+      <c r="A249" s="1">
         <v>14</v>
       </c>
       <c r="B249" t="s">
@@ -13590,7 +13583,7 @@
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A250">
+      <c r="A250" s="1">
         <v>15</v>
       </c>
       <c r="B250" t="s">
@@ -13613,7 +13606,7 @@
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A251">
+      <c r="A251" s="1">
         <v>16</v>
       </c>
       <c r="B251" t="s">
@@ -13636,7 +13629,7 @@
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A252">
+      <c r="A252" s="1">
         <v>17</v>
       </c>
       <c r="B252" t="s">
@@ -13659,7 +13652,7 @@
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253">
+      <c r="A253" s="1">
         <v>18</v>
       </c>
       <c r="B253" t="s">
@@ -13682,7 +13675,7 @@
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254">
+      <c r="A254" s="1">
         <v>19</v>
       </c>
       <c r="B254" t="s">
@@ -13705,7 +13698,7 @@
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A255">
+      <c r="A255" s="1">
         <v>20</v>
       </c>
       <c r="B255" t="s">
@@ -13728,7 +13721,7 @@
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A256">
+      <c r="A256" s="1">
         <v>21</v>
       </c>
       <c r="B256" t="s">
@@ -13751,7 +13744,7 @@
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A257">
+      <c r="A257" s="1">
         <v>22</v>
       </c>
       <c r="B257" t="s">
@@ -13774,7 +13767,7 @@
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A258">
+      <c r="A258" s="1">
         <v>23</v>
       </c>
       <c r="B258" t="s">
@@ -13797,7 +13790,7 @@
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A259">
+      <c r="A259" s="1">
         <v>24</v>
       </c>
       <c r="B259" t="s">
@@ -13820,7 +13813,7 @@
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A260">
+      <c r="A260" s="1">
         <v>25</v>
       </c>
       <c r="B260" t="s">
@@ -13857,7 +13850,7 @@
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A262">
+      <c r="A262" s="1">
         <v>1</v>
       </c>
       <c r="B262" t="s">
@@ -13880,7 +13873,7 @@
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A263">
+      <c r="A263" s="1">
         <v>2</v>
       </c>
       <c r="B263" t="s">
@@ -13903,7 +13896,7 @@
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A264">
+      <c r="A264" s="1">
         <v>3</v>
       </c>
       <c r="B264" t="s">
@@ -13926,7 +13919,7 @@
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A265">
+      <c r="A265" s="1">
         <v>4</v>
       </c>
       <c r="B265" t="s">
@@ -13949,7 +13942,7 @@
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A266">
+      <c r="A266" s="1">
         <v>5</v>
       </c>
       <c r="B266" t="s">
@@ -13972,7 +13965,7 @@
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A267">
+      <c r="A267" s="1">
         <v>6</v>
       </c>
       <c r="B267" t="s">
@@ -13995,7 +13988,7 @@
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A268">
+      <c r="A268" s="1">
         <v>7</v>
       </c>
       <c r="B268" t="s">
@@ -14018,7 +14011,7 @@
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269">
+      <c r="A269" s="1">
         <v>8</v>
       </c>
       <c r="B269" t="s">
@@ -14041,7 +14034,7 @@
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A270">
+      <c r="A270" s="1">
         <v>9</v>
       </c>
       <c r="B270" t="s">
@@ -14064,7 +14057,7 @@
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A271">
+      <c r="A271" s="1">
         <v>10</v>
       </c>
       <c r="B271" t="s">
@@ -14087,7 +14080,7 @@
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A272">
+      <c r="A272" s="1">
         <v>11</v>
       </c>
       <c r="B272" t="s">
@@ -14110,7 +14103,7 @@
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A273">
+      <c r="A273" s="1">
         <v>12</v>
       </c>
       <c r="B273" t="s">
@@ -14133,7 +14126,7 @@
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A274">
+      <c r="A274" s="1">
         <v>13</v>
       </c>
       <c r="B274" t="s">
@@ -14156,7 +14149,7 @@
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A275">
+      <c r="A275" s="1">
         <v>14</v>
       </c>
       <c r="B275" t="s">
@@ -14179,7 +14172,7 @@
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A276">
+      <c r="A276" s="1">
         <v>15</v>
       </c>
       <c r="B276" t="s">
@@ -14202,7 +14195,7 @@
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A277">
+      <c r="A277" s="1">
         <v>16</v>
       </c>
       <c r="B277" t="s">
@@ -14225,7 +14218,7 @@
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278">
+      <c r="A278" s="1">
         <v>17</v>
       </c>
       <c r="B278" t="s">
@@ -14248,7 +14241,7 @@
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A279">
+      <c r="A279" s="1">
         <v>18</v>
       </c>
       <c r="B279" t="s">
@@ -14271,7 +14264,7 @@
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A280">
+      <c r="A280" s="1">
         <v>19</v>
       </c>
       <c r="B280" t="s">
@@ -14294,7 +14287,7 @@
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A281">
+      <c r="A281" s="1">
         <v>20</v>
       </c>
       <c r="B281" t="s">
@@ -14317,7 +14310,7 @@
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A282">
+      <c r="A282" s="1">
         <v>21</v>
       </c>
       <c r="B282" t="s">
@@ -14340,7 +14333,7 @@
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A283">
+      <c r="A283" s="1">
         <v>22</v>
       </c>
       <c r="B283" t="s">
@@ -14363,7 +14356,7 @@
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A284">
+      <c r="A284" s="1">
         <v>23</v>
       </c>
       <c r="B284" t="s">
@@ -14386,7 +14379,7 @@
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A285">
+      <c r="A285" s="1">
         <v>24</v>
       </c>
       <c r="B285" t="s">
@@ -14409,7 +14402,7 @@
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286">
+      <c r="A286" s="1">
         <v>25</v>
       </c>
       <c r="B286" t="s">
@@ -14446,7 +14439,7 @@
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A288">
+      <c r="A288" s="1">
         <v>1</v>
       </c>
       <c r="B288" t="s">
@@ -14469,7 +14462,7 @@
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A289">
+      <c r="A289" s="1">
         <v>2</v>
       </c>
       <c r="B289" t="s">
@@ -14492,7 +14485,7 @@
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A290">
+      <c r="A290" s="1">
         <v>3</v>
       </c>
       <c r="B290" t="s">
@@ -14515,7 +14508,7 @@
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A291">
+      <c r="A291" s="1">
         <v>4</v>
       </c>
       <c r="B291" t="s">
@@ -14538,7 +14531,7 @@
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A292">
+      <c r="A292" s="1">
         <v>5</v>
       </c>
       <c r="B292" t="s">
@@ -14561,7 +14554,7 @@
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A293">
+      <c r="A293" s="1">
         <v>6</v>
       </c>
       <c r="B293" t="s">
@@ -14584,7 +14577,7 @@
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A294">
+      <c r="A294" s="1">
         <v>7</v>
       </c>
       <c r="B294" t="s">
@@ -14607,7 +14600,7 @@
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A295">
+      <c r="A295" s="1">
         <v>8</v>
       </c>
       <c r="B295" t="s">
@@ -14630,7 +14623,7 @@
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A296">
+      <c r="A296" s="1">
         <v>9</v>
       </c>
       <c r="B296" t="s">
@@ -14653,7 +14646,7 @@
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A297">
+      <c r="A297" s="1">
         <v>10</v>
       </c>
       <c r="B297" t="s">
@@ -14676,7 +14669,7 @@
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A298">
+      <c r="A298" s="1">
         <v>11</v>
       </c>
       <c r="B298" t="s">
@@ -14699,7 +14692,7 @@
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A299">
+      <c r="A299" s="1">
         <v>12</v>
       </c>
       <c r="B299" t="s">
@@ -14722,7 +14715,7 @@
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A300">
+      <c r="A300" s="1">
         <v>13</v>
       </c>
       <c r="B300" t="s">
@@ -14745,7 +14738,7 @@
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A301">
+      <c r="A301" s="1">
         <v>14</v>
       </c>
       <c r="B301" t="s">
@@ -14768,7 +14761,7 @@
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A302">
+      <c r="A302" s="1">
         <v>15</v>
       </c>
       <c r="B302" t="s">
@@ -14791,7 +14784,7 @@
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A303">
+      <c r="A303" s="1">
         <v>16</v>
       </c>
       <c r="B303" t="s">
@@ -14814,7 +14807,7 @@
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A304">
+      <c r="A304" s="1">
         <v>17</v>
       </c>
       <c r="B304" t="s">
@@ -14837,7 +14830,7 @@
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A305">
+      <c r="A305" s="1">
         <v>18</v>
       </c>
       <c r="B305" t="s">
@@ -14860,7 +14853,7 @@
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A306">
+      <c r="A306" s="1">
         <v>19</v>
       </c>
       <c r="B306" t="s">
@@ -14883,7 +14876,7 @@
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A307">
+      <c r="A307" s="1">
         <v>20</v>
       </c>
       <c r="B307" t="s">
@@ -14906,7 +14899,7 @@
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A308">
+      <c r="A308" s="1">
         <v>21</v>
       </c>
       <c r="B308" t="s">
@@ -14929,7 +14922,7 @@
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A309">
+      <c r="A309" s="1">
         <v>22</v>
       </c>
       <c r="B309" t="s">
@@ -14952,7 +14945,7 @@
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A310">
+      <c r="A310" s="1">
         <v>23</v>
       </c>
       <c r="B310" t="s">
@@ -14975,7 +14968,7 @@
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A311">
+      <c r="A311" s="1">
         <v>24</v>
       </c>
       <c r="B311" t="s">
@@ -14998,7 +14991,7 @@
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A312">
+      <c r="A312" s="1">
         <v>25</v>
       </c>
       <c r="B312" t="s">
@@ -15035,7 +15028,7 @@
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A314">
+      <c r="A314" s="1">
         <v>1</v>
       </c>
       <c r="B314" t="s">
@@ -15058,7 +15051,7 @@
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A315">
+      <c r="A315" s="1">
         <v>2</v>
       </c>
       <c r="B315" t="s">
@@ -15081,7 +15074,7 @@
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A316">
+      <c r="A316" s="1">
         <v>3</v>
       </c>
       <c r="B316" t="s">
@@ -15104,7 +15097,7 @@
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A317">
+      <c r="A317" s="1">
         <v>4</v>
       </c>
       <c r="B317" t="s">
@@ -15127,7 +15120,7 @@
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A318">
+      <c r="A318" s="1">
         <v>5</v>
       </c>
       <c r="B318" t="s">
@@ -15150,7 +15143,7 @@
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A319">
+      <c r="A319" s="1">
         <v>6</v>
       </c>
       <c r="B319" t="s">
@@ -15173,7 +15166,7 @@
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A320">
+      <c r="A320" s="1">
         <v>7</v>
       </c>
       <c r="B320" t="s">
@@ -15196,7 +15189,7 @@
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A321">
+      <c r="A321" s="1">
         <v>8</v>
       </c>
       <c r="B321" t="s">
@@ -15219,7 +15212,7 @@
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A322">
+      <c r="A322" s="1">
         <v>9</v>
       </c>
       <c r="B322" t="s">
@@ -15242,7 +15235,7 @@
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A323">
+      <c r="A323" s="1">
         <v>10</v>
       </c>
       <c r="B323" t="s">
@@ -15265,7 +15258,7 @@
       </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A324">
+      <c r="A324" s="1">
         <v>11</v>
       </c>
       <c r="B324" t="s">
@@ -15288,7 +15281,7 @@
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A325">
+      <c r="A325" s="1">
         <v>12</v>
       </c>
       <c r="B325" t="s">
@@ -15311,7 +15304,7 @@
       </c>
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A326">
+      <c r="A326" s="1">
         <v>13</v>
       </c>
       <c r="B326" t="s">
@@ -15334,7 +15327,7 @@
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A327">
+      <c r="A327" s="1">
         <v>14</v>
       </c>
       <c r="B327" t="s">
@@ -15357,7 +15350,7 @@
       </c>
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A328">
+      <c r="A328" s="1">
         <v>15</v>
       </c>
       <c r="B328" t="s">
@@ -15380,7 +15373,7 @@
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A329">
+      <c r="A329" s="1">
         <v>16</v>
       </c>
       <c r="B329" t="s">
@@ -15403,7 +15396,7 @@
       </c>
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A330">
+      <c r="A330" s="1">
         <v>17</v>
       </c>
       <c r="B330" t="s">
@@ -15426,7 +15419,7 @@
       </c>
     </row>
     <row r="331" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A331">
+      <c r="A331" s="1">
         <v>18</v>
       </c>
       <c r="B331" t="s">
@@ -15449,7 +15442,7 @@
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A332">
+      <c r="A332" s="1">
         <v>19</v>
       </c>
       <c r="B332" t="s">
@@ -15472,7 +15465,7 @@
       </c>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A333">
+      <c r="A333" s="1">
         <v>20</v>
       </c>
       <c r="B333" t="s">
@@ -15495,7 +15488,7 @@
       </c>
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A334">
+      <c r="A334" s="1">
         <v>21</v>
       </c>
       <c r="B334" t="s">
@@ -15518,7 +15511,7 @@
       </c>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A335">
+      <c r="A335" s="1">
         <v>22</v>
       </c>
       <c r="B335" t="s">
@@ -15541,7 +15534,7 @@
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A336">
+      <c r="A336" s="1">
         <v>23</v>
       </c>
       <c r="B336" t="s">
@@ -15564,7 +15557,7 @@
       </c>
     </row>
     <row r="337" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A337">
+      <c r="A337" s="1">
         <v>24</v>
       </c>
       <c r="B337" t="s">
@@ -15587,7 +15580,7 @@
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A338">
+      <c r="A338" s="1">
         <v>25</v>
       </c>
       <c r="B338" t="s">
@@ -15624,7 +15617,7 @@
       </c>
     </row>
     <row r="340" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A340">
+      <c r="A340" s="1">
         <v>1</v>
       </c>
       <c r="B340" t="s">
@@ -15647,7 +15640,7 @@
       </c>
     </row>
     <row r="341" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A341">
+      <c r="A341" s="1">
         <v>2</v>
       </c>
       <c r="B341" t="s">
@@ -15670,7 +15663,7 @@
       </c>
     </row>
     <row r="342" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A342">
+      <c r="A342" s="1">
         <v>3</v>
       </c>
       <c r="B342" t="s">
@@ -15693,7 +15686,7 @@
       </c>
     </row>
     <row r="343" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A343">
+      <c r="A343" s="1">
         <v>4</v>
       </c>
       <c r="B343" t="s">
@@ -15716,7 +15709,7 @@
       </c>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A344">
+      <c r="A344" s="1">
         <v>5</v>
       </c>
       <c r="B344" t="s">
@@ -15739,7 +15732,7 @@
       </c>
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A345">
+      <c r="A345" s="1">
         <v>6</v>
       </c>
       <c r="B345" t="s">
@@ -15762,7 +15755,7 @@
       </c>
     </row>
     <row r="346" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A346">
+      <c r="A346" s="1">
         <v>7</v>
       </c>
       <c r="B346" t="s">
@@ -15785,7 +15778,7 @@
       </c>
     </row>
     <row r="347" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A347">
+      <c r="A347" s="1">
         <v>8</v>
       </c>
       <c r="B347" t="s">
@@ -15808,7 +15801,7 @@
       </c>
     </row>
     <row r="348" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A348">
+      <c r="A348" s="1">
         <v>9</v>
       </c>
       <c r="B348" t="s">
@@ -15831,7 +15824,7 @@
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A349">
+      <c r="A349" s="1">
         <v>10</v>
       </c>
       <c r="B349" t="s">
@@ -15854,7 +15847,7 @@
       </c>
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A350">
+      <c r="A350" s="1">
         <v>11</v>
       </c>
       <c r="B350" t="s">
@@ -15877,7 +15870,7 @@
       </c>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A351">
+      <c r="A351" s="1">
         <v>12</v>
       </c>
       <c r="B351" t="s">
@@ -15900,7 +15893,7 @@
       </c>
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A352">
+      <c r="A352" s="1">
         <v>13</v>
       </c>
       <c r="B352" t="s">
@@ -15923,7 +15916,7 @@
       </c>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A353">
+      <c r="A353" s="1">
         <v>14</v>
       </c>
       <c r="B353" t="s">
@@ -15946,7 +15939,7 @@
       </c>
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A354">
+      <c r="A354" s="1">
         <v>15</v>
       </c>
       <c r="B354" t="s">
@@ -15969,7 +15962,7 @@
       </c>
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A355">
+      <c r="A355" s="1">
         <v>16</v>
       </c>
       <c r="B355" t="s">
@@ -15992,7 +15985,7 @@
       </c>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A356">
+      <c r="A356" s="1">
         <v>17</v>
       </c>
       <c r="B356" t="s">
@@ -16015,7 +16008,7 @@
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A357">
+      <c r="A357" s="1">
         <v>18</v>
       </c>
       <c r="B357" t="s">
@@ -16038,7 +16031,7 @@
       </c>
     </row>
     <row r="358" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A358">
+      <c r="A358" s="1">
         <v>19</v>
       </c>
       <c r="B358" t="s">
@@ -16061,7 +16054,7 @@
       </c>
     </row>
     <row r="359" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A359">
+      <c r="A359" s="1">
         <v>20</v>
       </c>
       <c r="B359" t="s">
@@ -16084,7 +16077,7 @@
       </c>
     </row>
     <row r="360" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A360">
+      <c r="A360" s="1">
         <v>21</v>
       </c>
       <c r="B360" t="s">
@@ -16107,7 +16100,7 @@
       </c>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A361">
+      <c r="A361" s="1">
         <v>22</v>
       </c>
       <c r="B361" t="s">
@@ -16130,7 +16123,7 @@
       </c>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A362">
+      <c r="A362" s="1">
         <v>23</v>
       </c>
       <c r="B362" t="s">
@@ -16153,7 +16146,7 @@
       </c>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A363">
+      <c r="A363" s="1">
         <v>24</v>
       </c>
       <c r="B363" t="s">
@@ -16176,7 +16169,7 @@
       </c>
     </row>
     <row r="364" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A364">
+      <c r="A364" s="1">
         <v>25</v>
       </c>
       <c r="B364" t="s">
@@ -16213,7 +16206,7 @@
       </c>
     </row>
     <row r="366" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A366">
+      <c r="A366" s="1">
         <v>1</v>
       </c>
       <c r="B366" t="s">
@@ -16236,7 +16229,7 @@
       </c>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A367">
+      <c r="A367" s="1">
         <v>2</v>
       </c>
       <c r="B367" t="s">
@@ -16259,7 +16252,7 @@
       </c>
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A368">
+      <c r="A368" s="1">
         <v>3</v>
       </c>
       <c r="B368" t="s">
@@ -16282,7 +16275,7 @@
       </c>
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A369">
+      <c r="A369" s="1">
         <v>4</v>
       </c>
       <c r="B369" t="s">
@@ -16305,7 +16298,7 @@
       </c>
     </row>
     <row r="370" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A370">
+      <c r="A370" s="1">
         <v>5</v>
       </c>
       <c r="B370" t="s">
@@ -16328,7 +16321,7 @@
       </c>
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A371">
+      <c r="A371" s="1">
         <v>6</v>
       </c>
       <c r="B371" t="s">
@@ -16351,7 +16344,7 @@
       </c>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A372">
+      <c r="A372" s="1">
         <v>7</v>
       </c>
       <c r="B372" t="s">
@@ -16374,7 +16367,7 @@
       </c>
     </row>
     <row r="373" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A373">
+      <c r="A373" s="1">
         <v>8</v>
       </c>
       <c r="B373" t="s">
@@ -16397,7 +16390,7 @@
       </c>
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A374">
+      <c r="A374" s="1">
         <v>9</v>
       </c>
       <c r="B374" t="s">
@@ -16420,7 +16413,7 @@
       </c>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A375">
+      <c r="A375" s="1">
         <v>10</v>
       </c>
       <c r="B375" t="s">
@@ -16443,7 +16436,7 @@
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A376">
+      <c r="A376" s="1">
         <v>11</v>
       </c>
       <c r="B376" t="s">
@@ -16466,7 +16459,7 @@
       </c>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A377">
+      <c r="A377" s="1">
         <v>12</v>
       </c>
       <c r="B377" t="s">
@@ -16489,7 +16482,7 @@
       </c>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A378">
+      <c r="A378" s="1">
         <v>13</v>
       </c>
       <c r="B378" t="s">
@@ -16512,7 +16505,7 @@
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A379">
+      <c r="A379" s="1">
         <v>14</v>
       </c>
       <c r="B379" t="s">
@@ -16535,7 +16528,7 @@
       </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A380">
+      <c r="A380" s="1">
         <v>15</v>
       </c>
       <c r="B380" t="s">
@@ -16558,7 +16551,7 @@
       </c>
     </row>
     <row r="381" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A381">
+      <c r="A381" s="1">
         <v>16</v>
       </c>
       <c r="B381" t="s">
@@ -16581,7 +16574,7 @@
       </c>
     </row>
     <row r="382" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A382">
+      <c r="A382" s="1">
         <v>17</v>
       </c>
       <c r="B382" t="s">
@@ -16604,7 +16597,7 @@
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A383">
+      <c r="A383" s="1">
         <v>18</v>
       </c>
       <c r="B383" t="s">
@@ -16627,7 +16620,7 @@
       </c>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A384">
+      <c r="A384" s="1">
         <v>19</v>
       </c>
       <c r="B384" t="s">
@@ -16650,7 +16643,7 @@
       </c>
     </row>
     <row r="385" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A385">
+      <c r="A385" s="1">
         <v>20</v>
       </c>
       <c r="B385" t="s">
@@ -16673,7 +16666,7 @@
       </c>
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A386">
+      <c r="A386" s="1">
         <v>21</v>
       </c>
       <c r="B386" t="s">
@@ -16696,7 +16689,7 @@
       </c>
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A387">
+      <c r="A387" s="1">
         <v>22</v>
       </c>
       <c r="B387" t="s">
@@ -16719,7 +16712,7 @@
       </c>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A388">
+      <c r="A388" s="1">
         <v>23</v>
       </c>
       <c r="B388" t="s">
@@ -16742,7 +16735,7 @@
       </c>
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A389">
+      <c r="A389" s="1">
         <v>24</v>
       </c>
       <c r="B389" t="s">
@@ -16765,7 +16758,7 @@
       </c>
     </row>
     <row r="390" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A390">
+      <c r="A390" s="1">
         <v>25</v>
       </c>
       <c r="B390" t="s">
@@ -16802,7 +16795,7 @@
       </c>
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A392">
+      <c r="A392" s="1">
         <v>1</v>
       </c>
       <c r="B392" t="s">
@@ -16825,7 +16818,7 @@
       </c>
     </row>
     <row r="393" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A393">
+      <c r="A393" s="1">
         <v>2</v>
       </c>
       <c r="B393" t="s">
@@ -16848,7 +16841,7 @@
       </c>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A394">
+      <c r="A394" s="1">
         <v>3</v>
       </c>
       <c r="B394" t="s">
@@ -16871,7 +16864,7 @@
       </c>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A395">
+      <c r="A395" s="1">
         <v>4</v>
       </c>
       <c r="B395" t="s">
@@ -16894,7 +16887,7 @@
       </c>
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A396">
+      <c r="A396" s="1">
         <v>5</v>
       </c>
       <c r="B396" t="s">
@@ -16917,7 +16910,7 @@
       </c>
     </row>
     <row r="397" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A397">
+      <c r="A397" s="1">
         <v>6</v>
       </c>
       <c r="B397" t="s">
@@ -16940,7 +16933,7 @@
       </c>
     </row>
     <row r="398" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A398">
+      <c r="A398" s="1">
         <v>7</v>
       </c>
       <c r="B398" t="s">
@@ -16963,7 +16956,7 @@
       </c>
     </row>
     <row r="399" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A399">
+      <c r="A399" s="1">
         <v>8</v>
       </c>
       <c r="B399" t="s">
@@ -16986,7 +16979,7 @@
       </c>
     </row>
     <row r="400" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A400">
+      <c r="A400" s="1">
         <v>9</v>
       </c>
       <c r="B400" t="s">
@@ -17009,7 +17002,7 @@
       </c>
     </row>
     <row r="401" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A401">
+      <c r="A401" s="1">
         <v>10</v>
       </c>
       <c r="B401" t="s">
@@ -17032,7 +17025,7 @@
       </c>
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A402">
+      <c r="A402" s="1">
         <v>11</v>
       </c>
       <c r="B402" t="s">
@@ -17055,7 +17048,7 @@
       </c>
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A403">
+      <c r="A403" s="1">
         <v>12</v>
       </c>
       <c r="B403" t="s">
@@ -17078,7 +17071,7 @@
       </c>
     </row>
     <row r="404" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A404">
+      <c r="A404" s="1">
         <v>13</v>
       </c>
       <c r="B404" t="s">
@@ -17101,7 +17094,7 @@
       </c>
     </row>
     <row r="405" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A405">
+      <c r="A405" s="1">
         <v>14</v>
       </c>
       <c r="B405" t="s">
@@ -17124,7 +17117,7 @@
       </c>
     </row>
     <row r="406" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A406">
+      <c r="A406" s="1">
         <v>15</v>
       </c>
       <c r="B406" t="s">
@@ -17147,7 +17140,7 @@
       </c>
     </row>
     <row r="407" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A407">
+      <c r="A407" s="1">
         <v>16</v>
       </c>
       <c r="B407" t="s">
@@ -17170,7 +17163,7 @@
       </c>
     </row>
     <row r="408" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A408">
+      <c r="A408" s="1">
         <v>17</v>
       </c>
       <c r="B408" t="s">
@@ -17193,7 +17186,7 @@
       </c>
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A409">
+      <c r="A409" s="1">
         <v>18</v>
       </c>
       <c r="B409" t="s">
@@ -17216,7 +17209,7 @@
       </c>
     </row>
     <row r="410" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A410">
+      <c r="A410" s="1">
         <v>19</v>
       </c>
       <c r="B410" t="s">
@@ -17239,7 +17232,7 @@
       </c>
     </row>
     <row r="411" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A411">
+      <c r="A411" s="1">
         <v>20</v>
       </c>
       <c r="B411" t="s">
@@ -17262,7 +17255,7 @@
       </c>
     </row>
     <row r="412" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A412">
+      <c r="A412" s="1">
         <v>21</v>
       </c>
       <c r="B412" t="s">
@@ -17285,7 +17278,7 @@
       </c>
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A413">
+      <c r="A413" s="1">
         <v>22</v>
       </c>
       <c r="B413" t="s">
@@ -17308,7 +17301,7 @@
       </c>
     </row>
     <row r="414" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A414">
+      <c r="A414" s="1">
         <v>23</v>
       </c>
       <c r="B414" t="s">
@@ -17331,7 +17324,7 @@
       </c>
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A415">
+      <c r="A415" s="1">
         <v>24</v>
       </c>
       <c r="B415" t="s">
@@ -17354,7 +17347,7 @@
       </c>
     </row>
     <row r="416" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A416">
+      <c r="A416" s="1">
         <v>25</v>
       </c>
       <c r="B416" t="s">
@@ -17991,7 +17984,6 @@
       </c>
     </row>
     <row r="443" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A443" s="1"/>
       <c r="B443" s="1"/>
       <c r="C443" s="1"/>
       <c r="D443" s="1" t="s">
@@ -18608,7 +18600,6 @@
       </c>
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A469" s="1"/>
       <c r="B469" s="1"/>
       <c r="C469" s="1"/>
       <c r="D469" s="1" t="s">
@@ -19225,7 +19216,6 @@
       </c>
     </row>
     <row r="495" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A495" s="1"/>
       <c r="B495" s="1"/>
       <c r="C495" s="1"/>
       <c r="D495" s="1" t="s">
@@ -19842,7 +19832,6 @@
       </c>
     </row>
     <row r="521" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A521" s="1"/>
       <c r="B521" s="1"/>
       <c r="C521" s="1"/>
       <c r="D521" s="1" t="s">
@@ -20459,7 +20448,6 @@
       </c>
     </row>
     <row r="547" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A547" s="1"/>
       <c r="B547" s="1"/>
       <c r="C547" s="1"/>
       <c r="D547" s="1" t="s">
@@ -21076,7 +21064,6 @@
       </c>
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A573" s="1"/>
       <c r="B573" s="1"/>
       <c r="C573" s="1"/>
       <c r="D573" s="1" t="s">
@@ -21093,7 +21080,7 @@
       </c>
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A574">
+      <c r="A574" s="1">
         <v>1</v>
       </c>
       <c r="B574" t="s">
@@ -21116,7 +21103,7 @@
       </c>
     </row>
     <row r="575" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A575" t="s">
+      <c r="A575" s="1" t="s">
         <v>1069</v>
       </c>
       <c r="B575" t="s">
@@ -21139,7 +21126,7 @@
       </c>
     </row>
     <row r="576" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A576">
+      <c r="A576" s="1">
         <v>2</v>
       </c>
       <c r="B576" t="s">
@@ -21162,7 +21149,7 @@
       </c>
     </row>
     <row r="577" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A577" t="s">
+      <c r="A577" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B577" t="s">
@@ -21185,7 +21172,7 @@
       </c>
     </row>
     <row r="578" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A578">
+      <c r="A578" s="1">
         <v>3</v>
       </c>
       <c r="B578" t="s">
@@ -21208,7 +21195,7 @@
       </c>
     </row>
     <row r="579" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A579" t="s">
+      <c r="A579" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="B579" t="s">
@@ -21231,7 +21218,7 @@
       </c>
     </row>
     <row r="580" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A580">
+      <c r="A580" s="1">
         <v>4</v>
       </c>
       <c r="B580" t="s">
@@ -21254,7 +21241,7 @@
       </c>
     </row>
     <row r="581" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A581" t="s">
+      <c r="A581" s="1" t="s">
         <v>1091</v>
       </c>
       <c r="B581" t="s">
@@ -21277,7 +21264,7 @@
       </c>
     </row>
     <row r="582" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A582">
+      <c r="A582" s="1">
         <v>5</v>
       </c>
       <c r="B582" t="s">
@@ -21300,7 +21287,7 @@
       </c>
     </row>
     <row r="583" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A583" t="s">
+      <c r="A583" s="1" t="s">
         <v>1098</v>
       </c>
       <c r="B583" t="s">
@@ -21323,7 +21310,7 @@
       </c>
     </row>
     <row r="584" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A584">
+      <c r="A584" s="1">
         <v>6</v>
       </c>
       <c r="B584" t="s">
@@ -21346,7 +21333,7 @@
       </c>
     </row>
     <row r="585" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A585" t="s">
+      <c r="A585" s="1" t="s">
         <v>1105</v>
       </c>
       <c r="B585" t="s">
@@ -21369,7 +21356,7 @@
       </c>
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A586">
+      <c r="A586" s="1">
         <v>7</v>
       </c>
       <c r="B586" t="s">
@@ -21392,7 +21379,7 @@
       </c>
     </row>
     <row r="587" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A587" t="s">
+      <c r="A587" s="1" t="s">
         <v>1112</v>
       </c>
       <c r="B587" t="s">
@@ -21415,7 +21402,7 @@
       </c>
     </row>
     <row r="588" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A588">
+      <c r="A588" s="1">
         <v>8</v>
       </c>
       <c r="B588" t="s">
@@ -21438,7 +21425,7 @@
       </c>
     </row>
     <row r="589" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A589" t="s">
+      <c r="A589" s="1" t="s">
         <v>1119</v>
       </c>
       <c r="B589" t="s">
@@ -21461,7 +21448,7 @@
       </c>
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A590">
+      <c r="A590" s="1">
         <v>9</v>
       </c>
       <c r="B590" t="s">
@@ -21484,7 +21471,7 @@
       </c>
     </row>
     <row r="591" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A591" t="s">
+      <c r="A591" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="B591" t="s">
@@ -21507,7 +21494,7 @@
       </c>
     </row>
     <row r="592" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A592">
+      <c r="A592" s="1">
         <v>10</v>
       </c>
       <c r="B592" t="s">
@@ -21530,7 +21517,7 @@
       </c>
     </row>
     <row r="593" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A593" t="s">
+      <c r="A593" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="B593" t="s">
@@ -21553,7 +21540,7 @@
       </c>
     </row>
     <row r="594" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A594">
+      <c r="A594" s="1">
         <v>11</v>
       </c>
       <c r="B594" t="s">
@@ -21576,7 +21563,7 @@
       </c>
     </row>
     <row r="595" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A595" t="s">
+      <c r="A595" s="1" t="s">
         <v>1140</v>
       </c>
       <c r="B595" t="s">
@@ -21599,7 +21586,7 @@
       </c>
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A596">
+      <c r="A596" s="1">
         <v>12</v>
       </c>
       <c r="B596" t="s">
@@ -21622,7 +21609,7 @@
       </c>
     </row>
     <row r="597" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A597" t="s">
+      <c r="A597" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B597" t="s">
@@ -21645,7 +21632,7 @@
       </c>
     </row>
     <row r="598" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A598">
+      <c r="A598" s="1">
         <v>13</v>
       </c>
       <c r="B598" t="s">
@@ -21682,7 +21669,7 @@
       </c>
     </row>
     <row r="600" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A600">
+      <c r="A600" s="1">
         <v>1</v>
       </c>
       <c r="B600" t="s">
@@ -21705,7 +21692,7 @@
       </c>
     </row>
     <row r="601" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A601" t="s">
+      <c r="A601" s="1" t="s">
         <v>1069</v>
       </c>
       <c r="B601" t="s">
@@ -21728,7 +21715,7 @@
       </c>
     </row>
     <row r="602" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A602">
+      <c r="A602" s="1">
         <v>2</v>
       </c>
       <c r="B602" t="s">
@@ -21751,7 +21738,7 @@
       </c>
     </row>
     <row r="603" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A603" t="s">
+      <c r="A603" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B603" t="s">
@@ -21774,7 +21761,7 @@
       </c>
     </row>
     <row r="604" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A604">
+      <c r="A604" s="1">
         <v>3</v>
       </c>
       <c r="B604" t="s">
@@ -21797,7 +21784,7 @@
       </c>
     </row>
     <row r="605" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A605" t="s">
+      <c r="A605" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="B605" t="s">
@@ -21820,7 +21807,7 @@
       </c>
     </row>
     <row r="606" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A606">
+      <c r="A606" s="1">
         <v>4</v>
       </c>
       <c r="B606" t="s">
@@ -21843,7 +21830,7 @@
       </c>
     </row>
     <row r="607" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A607" t="s">
+      <c r="A607" s="1" t="s">
         <v>1091</v>
       </c>
       <c r="B607" t="s">
@@ -21866,7 +21853,7 @@
       </c>
     </row>
     <row r="608" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A608">
+      <c r="A608" s="1">
         <v>5</v>
       </c>
       <c r="B608" t="s">
@@ -21889,7 +21876,7 @@
       </c>
     </row>
     <row r="609" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A609" t="s">
+      <c r="A609" s="1" t="s">
         <v>1098</v>
       </c>
       <c r="B609" t="s">
@@ -21912,7 +21899,7 @@
       </c>
     </row>
     <row r="610" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A610">
+      <c r="A610" s="1">
         <v>6</v>
       </c>
       <c r="B610" t="s">
@@ -21935,7 +21922,7 @@
       </c>
     </row>
     <row r="611" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A611" t="s">
+      <c r="A611" s="1" t="s">
         <v>1105</v>
       </c>
       <c r="B611" t="s">
@@ -21958,7 +21945,7 @@
       </c>
     </row>
     <row r="612" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A612">
+      <c r="A612" s="1">
         <v>7</v>
       </c>
       <c r="B612" t="s">
@@ -21981,7 +21968,7 @@
       </c>
     </row>
     <row r="613" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A613" t="s">
+      <c r="A613" s="1" t="s">
         <v>1112</v>
       </c>
       <c r="B613" t="s">
@@ -22004,7 +21991,7 @@
       </c>
     </row>
     <row r="614" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A614">
+      <c r="A614" s="1">
         <v>8</v>
       </c>
       <c r="B614" t="s">
@@ -22027,7 +22014,7 @@
       </c>
     </row>
     <row r="615" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A615" t="s">
+      <c r="A615" s="1" t="s">
         <v>1119</v>
       </c>
       <c r="B615" t="s">
@@ -22050,7 +22037,7 @@
       </c>
     </row>
     <row r="616" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A616">
+      <c r="A616" s="1">
         <v>9</v>
       </c>
       <c r="B616" t="s">
@@ -22073,7 +22060,7 @@
       </c>
     </row>
     <row r="617" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A617" t="s">
+      <c r="A617" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="B617" t="s">
@@ -22096,7 +22083,7 @@
       </c>
     </row>
     <row r="618" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A618">
+      <c r="A618" s="1">
         <v>10</v>
       </c>
       <c r="B618" t="s">
@@ -22119,7 +22106,7 @@
       </c>
     </row>
     <row r="619" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A619" t="s">
+      <c r="A619" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="B619" t="s">
@@ -22142,7 +22129,7 @@
       </c>
     </row>
     <row r="620" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A620">
+      <c r="A620" s="1">
         <v>11</v>
       </c>
       <c r="B620" t="s">
@@ -22165,7 +22152,7 @@
       </c>
     </row>
     <row r="621" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A621" t="s">
+      <c r="A621" s="1" t="s">
         <v>1140</v>
       </c>
       <c r="B621" t="s">
@@ -22188,7 +22175,7 @@
       </c>
     </row>
     <row r="622" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A622">
+      <c r="A622" s="1">
         <v>12</v>
       </c>
       <c r="B622" t="s">
@@ -22211,7 +22198,7 @@
       </c>
     </row>
     <row r="623" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A623" t="s">
+      <c r="A623" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B623" t="s">
@@ -22234,7 +22221,7 @@
       </c>
     </row>
     <row r="624" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A624">
+      <c r="A624" s="1">
         <v>13</v>
       </c>
       <c r="B624" t="s">
@@ -22271,7 +22258,7 @@
       </c>
     </row>
     <row r="626" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A626">
+      <c r="A626" s="1">
         <v>1</v>
       </c>
       <c r="B626" t="s">
@@ -22294,7 +22281,7 @@
       </c>
     </row>
     <row r="627" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A627" t="s">
+      <c r="A627" s="1" t="s">
         <v>1069</v>
       </c>
       <c r="B627" t="s">
@@ -22317,7 +22304,7 @@
       </c>
     </row>
     <row r="628" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A628">
+      <c r="A628" s="1">
         <v>2</v>
       </c>
       <c r="B628" t="s">
@@ -22340,7 +22327,7 @@
       </c>
     </row>
     <row r="629" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A629" t="s">
+      <c r="A629" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B629" t="s">
@@ -22363,7 +22350,7 @@
       </c>
     </row>
     <row r="630" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A630">
+      <c r="A630" s="1">
         <v>3</v>
       </c>
       <c r="B630" t="s">
@@ -22386,7 +22373,7 @@
       </c>
     </row>
     <row r="631" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A631" t="s">
+      <c r="A631" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="B631" t="s">
@@ -22409,7 +22396,7 @@
       </c>
     </row>
     <row r="632" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A632">
+      <c r="A632" s="1">
         <v>4</v>
       </c>
       <c r="B632" t="s">
@@ -22432,7 +22419,7 @@
       </c>
     </row>
     <row r="633" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A633" t="s">
+      <c r="A633" s="1" t="s">
         <v>1091</v>
       </c>
       <c r="B633" t="s">
@@ -22455,7 +22442,7 @@
       </c>
     </row>
     <row r="634" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A634">
+      <c r="A634" s="1">
         <v>5</v>
       </c>
       <c r="B634" t="s">
@@ -22478,7 +22465,7 @@
       </c>
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A635" t="s">
+      <c r="A635" s="1" t="s">
         <v>1098</v>
       </c>
       <c r="B635" t="s">
@@ -22501,7 +22488,7 @@
       </c>
     </row>
     <row r="636" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A636">
+      <c r="A636" s="1">
         <v>6</v>
       </c>
       <c r="B636" t="s">
@@ -22524,7 +22511,7 @@
       </c>
     </row>
     <row r="637" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A637" t="s">
+      <c r="A637" s="1" t="s">
         <v>1105</v>
       </c>
       <c r="B637" t="s">
@@ -22547,7 +22534,7 @@
       </c>
     </row>
     <row r="638" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A638">
+      <c r="A638" s="1">
         <v>7</v>
       </c>
       <c r="B638" t="s">
@@ -22570,7 +22557,7 @@
       </c>
     </row>
     <row r="639" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A639" t="s">
+      <c r="A639" s="1" t="s">
         <v>1112</v>
       </c>
       <c r="B639" t="s">
@@ -22593,7 +22580,7 @@
       </c>
     </row>
     <row r="640" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A640">
+      <c r="A640" s="1">
         <v>8</v>
       </c>
       <c r="B640" t="s">
@@ -22616,7 +22603,7 @@
       </c>
     </row>
     <row r="641" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A641" t="s">
+      <c r="A641" s="1" t="s">
         <v>1119</v>
       </c>
       <c r="B641" t="s">
@@ -22639,7 +22626,7 @@
       </c>
     </row>
     <row r="642" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A642">
+      <c r="A642" s="1">
         <v>9</v>
       </c>
       <c r="B642" t="s">
@@ -22662,7 +22649,7 @@
       </c>
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A643" t="s">
+      <c r="A643" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="B643" t="s">
@@ -22685,7 +22672,7 @@
       </c>
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A644">
+      <c r="A644" s="1">
         <v>10</v>
       </c>
       <c r="B644" t="s">
@@ -22708,7 +22695,7 @@
       </c>
     </row>
     <row r="645" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A645" t="s">
+      <c r="A645" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="B645" t="s">
@@ -22731,7 +22718,7 @@
       </c>
     </row>
     <row r="646" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A646">
+      <c r="A646" s="1">
         <v>11</v>
       </c>
       <c r="B646" t="s">
@@ -22754,7 +22741,7 @@
       </c>
     </row>
     <row r="647" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A647" t="s">
+      <c r="A647" s="1" t="s">
         <v>1140</v>
       </c>
       <c r="B647" t="s">
@@ -22777,7 +22764,7 @@
       </c>
     </row>
     <row r="648" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A648">
+      <c r="A648" s="1">
         <v>12</v>
       </c>
       <c r="B648" t="s">
@@ -22800,7 +22787,7 @@
       </c>
     </row>
     <row r="649" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A649" t="s">
+      <c r="A649" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B649" t="s">
@@ -22823,7 +22810,7 @@
       </c>
     </row>
     <row r="650" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A650">
+      <c r="A650" s="1">
         <v>13</v>
       </c>
       <c r="B650" t="s">
@@ -22860,7 +22847,7 @@
       </c>
     </row>
     <row r="652" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A652">
+      <c r="A652" s="1">
         <v>1</v>
       </c>
       <c r="B652" t="s">
@@ -22883,7 +22870,7 @@
       </c>
     </row>
     <row r="653" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A653" t="s">
+      <c r="A653" s="1" t="s">
         <v>1069</v>
       </c>
       <c r="B653" t="s">
@@ -22906,7 +22893,7 @@
       </c>
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A654">
+      <c r="A654" s="1">
         <v>2</v>
       </c>
       <c r="B654" t="s">
@@ -22929,7 +22916,7 @@
       </c>
     </row>
     <row r="655" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A655" t="s">
+      <c r="A655" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B655" t="s">
@@ -22952,7 +22939,7 @@
       </c>
     </row>
     <row r="656" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A656">
+      <c r="A656" s="1">
         <v>3</v>
       </c>
       <c r="B656" t="s">
@@ -22975,7 +22962,7 @@
       </c>
     </row>
     <row r="657" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A657" t="s">
+      <c r="A657" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="B657" t="s">
@@ -22998,7 +22985,7 @@
       </c>
     </row>
     <row r="658" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A658">
+      <c r="A658" s="1">
         <v>4</v>
       </c>
       <c r="B658" t="s">
@@ -23021,7 +23008,7 @@
       </c>
     </row>
     <row r="659" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A659" t="s">
+      <c r="A659" s="1" t="s">
         <v>1091</v>
       </c>
       <c r="B659" t="s">
@@ -23044,7 +23031,7 @@
       </c>
     </row>
     <row r="660" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A660">
+      <c r="A660" s="1">
         <v>5</v>
       </c>
       <c r="B660" t="s">
@@ -23067,7 +23054,7 @@
       </c>
     </row>
     <row r="661" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A661" t="s">
+      <c r="A661" s="1" t="s">
         <v>1098</v>
       </c>
       <c r="B661" t="s">
@@ -23090,7 +23077,7 @@
       </c>
     </row>
     <row r="662" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A662">
+      <c r="A662" s="1">
         <v>6</v>
       </c>
       <c r="B662" t="s">
@@ -23113,7 +23100,7 @@
       </c>
     </row>
     <row r="663" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A663" t="s">
+      <c r="A663" s="1" t="s">
         <v>1105</v>
       </c>
       <c r="B663" t="s">
@@ -23136,7 +23123,7 @@
       </c>
     </row>
     <row r="664" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A664">
+      <c r="A664" s="1">
         <v>7</v>
       </c>
       <c r="B664" t="s">
@@ -23159,7 +23146,7 @@
       </c>
     </row>
     <row r="665" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A665" t="s">
+      <c r="A665" s="1" t="s">
         <v>1112</v>
       </c>
       <c r="B665" t="s">
@@ -23182,7 +23169,7 @@
       </c>
     </row>
     <row r="666" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A666">
+      <c r="A666" s="1">
         <v>8</v>
       </c>
       <c r="B666" t="s">
@@ -23205,7 +23192,7 @@
       </c>
     </row>
     <row r="667" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A667" t="s">
+      <c r="A667" s="1" t="s">
         <v>1119</v>
       </c>
       <c r="B667" t="s">
@@ -23228,7 +23215,7 @@
       </c>
     </row>
     <row r="668" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A668">
+      <c r="A668" s="1">
         <v>9</v>
       </c>
       <c r="B668" t="s">
@@ -23251,7 +23238,7 @@
       </c>
     </row>
     <row r="669" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A669" t="s">
+      <c r="A669" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="B669" t="s">
@@ -23274,7 +23261,7 @@
       </c>
     </row>
     <row r="670" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A670">
+      <c r="A670" s="1">
         <v>10</v>
       </c>
       <c r="B670" t="s">
@@ -23297,7 +23284,7 @@
       </c>
     </row>
     <row r="671" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A671" t="s">
+      <c r="A671" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="B671" t="s">
@@ -23320,7 +23307,7 @@
       </c>
     </row>
     <row r="672" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A672">
+      <c r="A672" s="1">
         <v>11</v>
       </c>
       <c r="B672" t="s">
@@ -23343,7 +23330,7 @@
       </c>
     </row>
     <row r="673" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A673" t="s">
+      <c r="A673" s="1" t="s">
         <v>1140</v>
       </c>
       <c r="B673" t="s">
@@ -23366,7 +23353,7 @@
       </c>
     </row>
     <row r="674" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A674">
+      <c r="A674" s="1">
         <v>12</v>
       </c>
       <c r="B674" t="s">
@@ -23389,7 +23376,7 @@
       </c>
     </row>
     <row r="675" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A675" t="s">
+      <c r="A675" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B675" t="s">
@@ -23412,7 +23399,7 @@
       </c>
     </row>
     <row r="676" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A676">
+      <c r="A676" s="1">
         <v>13</v>
       </c>
       <c r="B676" t="s">
@@ -23449,7 +23436,7 @@
       </c>
     </row>
     <row r="678" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A678">
+      <c r="A678" s="1">
         <v>1</v>
       </c>
       <c r="B678" t="s">
@@ -23472,7 +23459,7 @@
       </c>
     </row>
     <row r="679" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A679" t="s">
+      <c r="A679" s="1" t="s">
         <v>1069</v>
       </c>
       <c r="B679" t="s">
@@ -23495,7 +23482,7 @@
       </c>
     </row>
     <row r="680" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A680">
+      <c r="A680" s="1">
         <v>2</v>
       </c>
       <c r="B680" t="s">
@@ -23518,7 +23505,7 @@
       </c>
     </row>
     <row r="681" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A681" t="s">
+      <c r="A681" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B681" t="s">
@@ -23541,7 +23528,7 @@
       </c>
     </row>
     <row r="682" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A682">
+      <c r="A682" s="1">
         <v>3</v>
       </c>
       <c r="B682" t="s">
@@ -23564,7 +23551,7 @@
       </c>
     </row>
     <row r="683" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A683" t="s">
+      <c r="A683" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="B683" t="s">
@@ -23587,7 +23574,7 @@
       </c>
     </row>
     <row r="684" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A684">
+      <c r="A684" s="1">
         <v>4</v>
       </c>
       <c r="B684" t="s">
@@ -23610,7 +23597,7 @@
       </c>
     </row>
     <row r="685" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A685" t="s">
+      <c r="A685" s="1" t="s">
         <v>1091</v>
       </c>
       <c r="B685" t="s">
@@ -23633,7 +23620,7 @@
       </c>
     </row>
     <row r="686" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A686">
+      <c r="A686" s="1">
         <v>5</v>
       </c>
       <c r="B686" t="s">
@@ -23656,7 +23643,7 @@
       </c>
     </row>
     <row r="687" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A687" t="s">
+      <c r="A687" s="1" t="s">
         <v>1098</v>
       </c>
       <c r="B687" t="s">
@@ -23679,7 +23666,7 @@
       </c>
     </row>
     <row r="688" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A688">
+      <c r="A688" s="1">
         <v>6</v>
       </c>
       <c r="B688" t="s">
@@ -23702,7 +23689,7 @@
       </c>
     </row>
     <row r="689" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A689" t="s">
+      <c r="A689" s="1" t="s">
         <v>1105</v>
       </c>
       <c r="B689" t="s">
@@ -23725,7 +23712,7 @@
       </c>
     </row>
     <row r="690" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A690">
+      <c r="A690" s="1">
         <v>7</v>
       </c>
       <c r="B690" t="s">
@@ -23748,7 +23735,7 @@
       </c>
     </row>
     <row r="691" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A691" t="s">
+      <c r="A691" s="1" t="s">
         <v>1112</v>
       </c>
       <c r="B691" t="s">
@@ -23771,7 +23758,7 @@
       </c>
     </row>
     <row r="692" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A692">
+      <c r="A692" s="1">
         <v>8</v>
       </c>
       <c r="B692" t="s">
@@ -23794,7 +23781,7 @@
       </c>
     </row>
     <row r="693" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A693" t="s">
+      <c r="A693" s="1" t="s">
         <v>1119</v>
       </c>
       <c r="B693" t="s">
@@ -23817,7 +23804,7 @@
       </c>
     </row>
     <row r="694" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A694">
+      <c r="A694" s="1">
         <v>9</v>
       </c>
       <c r="B694" t="s">
@@ -23840,7 +23827,7 @@
       </c>
     </row>
     <row r="695" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A695" t="s">
+      <c r="A695" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="B695" t="s">
@@ -23863,7 +23850,7 @@
       </c>
     </row>
     <row r="696" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A696">
+      <c r="A696" s="1">
         <v>10</v>
       </c>
       <c r="B696" t="s">
@@ -23886,7 +23873,7 @@
       </c>
     </row>
     <row r="697" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A697" t="s">
+      <c r="A697" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="B697" t="s">
@@ -23909,7 +23896,7 @@
       </c>
     </row>
     <row r="698" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A698">
+      <c r="A698" s="1">
         <v>11</v>
       </c>
       <c r="B698" t="s">
@@ -23932,7 +23919,7 @@
       </c>
     </row>
     <row r="699" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A699" t="s">
+      <c r="A699" s="1" t="s">
         <v>1140</v>
       </c>
       <c r="B699" t="s">
@@ -23955,7 +23942,7 @@
       </c>
     </row>
     <row r="700" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A700">
+      <c r="A700" s="1">
         <v>12</v>
       </c>
       <c r="B700" t="s">
@@ -23978,7 +23965,7 @@
       </c>
     </row>
     <row r="701" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A701" t="s">
+      <c r="A701" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B701" t="s">
@@ -24001,7 +23988,7 @@
       </c>
     </row>
     <row r="702" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A702">
+      <c r="A702" s="1">
         <v>13</v>
       </c>
       <c r="B702" t="s">
@@ -24038,7 +24025,7 @@
       </c>
     </row>
     <row r="704" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A704">
+      <c r="A704" s="1">
         <v>1</v>
       </c>
       <c r="B704" t="s">
@@ -24061,7 +24048,7 @@
       </c>
     </row>
     <row r="705" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A705" t="s">
+      <c r="A705" s="1" t="s">
         <v>1069</v>
       </c>
       <c r="B705" t="s">
@@ -24084,7 +24071,7 @@
       </c>
     </row>
     <row r="706" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A706">
+      <c r="A706" s="1">
         <v>2</v>
       </c>
       <c r="B706" t="s">
@@ -24107,7 +24094,7 @@
       </c>
     </row>
     <row r="707" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A707" t="s">
+      <c r="A707" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B707" t="s">
@@ -24130,7 +24117,7 @@
       </c>
     </row>
     <row r="708" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A708">
+      <c r="A708" s="1">
         <v>3</v>
       </c>
       <c r="B708" t="s">
@@ -24153,7 +24140,7 @@
       </c>
     </row>
     <row r="709" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A709" t="s">
+      <c r="A709" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="B709" t="s">
@@ -24176,7 +24163,7 @@
       </c>
     </row>
     <row r="710" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A710">
+      <c r="A710" s="1">
         <v>4</v>
       </c>
       <c r="B710" t="s">
@@ -24199,7 +24186,7 @@
       </c>
     </row>
     <row r="711" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A711" t="s">
+      <c r="A711" s="1" t="s">
         <v>1091</v>
       </c>
       <c r="B711" t="s">
@@ -24222,7 +24209,7 @@
       </c>
     </row>
     <row r="712" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A712">
+      <c r="A712" s="1">
         <v>5</v>
       </c>
       <c r="B712" t="s">
@@ -24245,7 +24232,7 @@
       </c>
     </row>
     <row r="713" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A713" t="s">
+      <c r="A713" s="1" t="s">
         <v>1098</v>
       </c>
       <c r="B713" t="s">
@@ -24268,7 +24255,7 @@
       </c>
     </row>
     <row r="714" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A714">
+      <c r="A714" s="1">
         <v>6</v>
       </c>
       <c r="B714" t="s">
@@ -24291,7 +24278,7 @@
       </c>
     </row>
     <row r="715" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A715" t="s">
+      <c r="A715" s="1" t="s">
         <v>1105</v>
       </c>
       <c r="B715" t="s">
@@ -24314,7 +24301,7 @@
       </c>
     </row>
     <row r="716" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A716">
+      <c r="A716" s="1">
         <v>7</v>
       </c>
       <c r="B716" t="s">
@@ -24337,7 +24324,7 @@
       </c>
     </row>
     <row r="717" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A717" t="s">
+      <c r="A717" s="1" t="s">
         <v>1112</v>
       </c>
       <c r="B717" t="s">
@@ -24360,7 +24347,7 @@
       </c>
     </row>
     <row r="718" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A718">
+      <c r="A718" s="1">
         <v>8</v>
       </c>
       <c r="B718" t="s">
@@ -24383,7 +24370,7 @@
       </c>
     </row>
     <row r="719" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A719" t="s">
+      <c r="A719" s="1" t="s">
         <v>1119</v>
       </c>
       <c r="B719" t="s">
@@ -24406,7 +24393,7 @@
       </c>
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A720">
+      <c r="A720" s="1">
         <v>9</v>
       </c>
       <c r="B720" t="s">
@@ -24429,7 +24416,7 @@
       </c>
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A721" t="s">
+      <c r="A721" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="B721" t="s">
@@ -24452,7 +24439,7 @@
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A722">
+      <c r="A722" s="1">
         <v>10</v>
       </c>
       <c r="B722" t="s">
@@ -24475,7 +24462,7 @@
       </c>
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A723" t="s">
+      <c r="A723" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="B723" t="s">
@@ -24498,7 +24485,7 @@
       </c>
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A724">
+      <c r="A724" s="1">
         <v>11</v>
       </c>
       <c r="B724" t="s">
@@ -24521,7 +24508,7 @@
       </c>
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A725" t="s">
+      <c r="A725" s="1" t="s">
         <v>1140</v>
       </c>
       <c r="B725" t="s">
@@ -24544,7 +24531,7 @@
       </c>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A726">
+      <c r="A726" s="1">
         <v>12</v>
       </c>
       <c r="B726" t="s">
@@ -24567,7 +24554,7 @@
       </c>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A727" t="s">
+      <c r="A727" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B727" t="s">
@@ -24590,7 +24577,7 @@
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A728">
+      <c r="A728" s="1">
         <v>13</v>
       </c>
       <c r="B728" t="s">
@@ -25202,7 +25189,6 @@
       </c>
     </row>
     <row r="755" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A755" s="1"/>
       <c r="B755" s="1"/>
       <c r="C755" s="1"/>
       <c r="D755" s="1" t="s">
@@ -25219,7 +25205,7 @@
       </c>
     </row>
     <row r="756" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A756">
+      <c r="A756" s="1">
         <v>1</v>
       </c>
       <c r="B756" t="s">
@@ -25242,7 +25228,7 @@
       </c>
     </row>
     <row r="757" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A757" t="s">
+      <c r="A757" s="1" t="s">
         <v>1069</v>
       </c>
       <c r="B757" t="s">
@@ -25265,7 +25251,7 @@
       </c>
     </row>
     <row r="758" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A758">
+      <c r="A758" s="1">
         <v>2</v>
       </c>
       <c r="B758" t="s">
@@ -25288,7 +25274,7 @@
       </c>
     </row>
     <row r="759" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A759" t="s">
+      <c r="A759" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B759" t="s">
@@ -25311,7 +25297,7 @@
       </c>
     </row>
     <row r="760" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A760">
+      <c r="A760" s="1">
         <v>3</v>
       </c>
       <c r="B760" t="s">
@@ -25334,7 +25320,7 @@
       </c>
     </row>
     <row r="761" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A761" t="s">
+      <c r="A761" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="B761" t="s">
@@ -25357,7 +25343,7 @@
       </c>
     </row>
     <row r="762" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A762">
+      <c r="A762" s="1">
         <v>4</v>
       </c>
       <c r="B762" t="s">
@@ -25380,7 +25366,7 @@
       </c>
     </row>
     <row r="763" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A763" t="s">
+      <c r="A763" s="1" t="s">
         <v>1091</v>
       </c>
       <c r="B763" t="s">
@@ -25403,7 +25389,7 @@
       </c>
     </row>
     <row r="764" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A764">
+      <c r="A764" s="1">
         <v>5</v>
       </c>
       <c r="B764" t="s">
@@ -25426,7 +25412,7 @@
       </c>
     </row>
     <row r="765" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A765" t="s">
+      <c r="A765" s="1" t="s">
         <v>1098</v>
       </c>
       <c r="B765" t="s">
@@ -25449,7 +25435,7 @@
       </c>
     </row>
     <row r="766" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A766">
+      <c r="A766" s="1">
         <v>6</v>
       </c>
       <c r="B766" t="s">
@@ -25472,7 +25458,7 @@
       </c>
     </row>
     <row r="767" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A767" t="s">
+      <c r="A767" s="1" t="s">
         <v>1105</v>
       </c>
       <c r="B767" t="s">
@@ -25495,7 +25481,7 @@
       </c>
     </row>
     <row r="768" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A768">
+      <c r="A768" s="1">
         <v>7</v>
       </c>
       <c r="B768" t="s">
@@ -25518,7 +25504,7 @@
       </c>
     </row>
     <row r="769" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A769" t="s">
+      <c r="A769" s="1" t="s">
         <v>1112</v>
       </c>
       <c r="B769" t="s">
@@ -25541,7 +25527,7 @@
       </c>
     </row>
     <row r="770" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A770">
+      <c r="A770" s="1">
         <v>8</v>
       </c>
       <c r="B770" t="s">
@@ -25564,7 +25550,7 @@
       </c>
     </row>
     <row r="771" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A771" t="s">
+      <c r="A771" s="1" t="s">
         <v>1119</v>
       </c>
       <c r="B771" t="s">
@@ -25587,7 +25573,7 @@
       </c>
     </row>
     <row r="772" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A772">
+      <c r="A772" s="1">
         <v>9</v>
       </c>
       <c r="B772" t="s">
@@ -25610,7 +25596,7 @@
       </c>
     </row>
     <row r="773" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A773" t="s">
+      <c r="A773" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="B773" t="s">
@@ -25633,7 +25619,7 @@
       </c>
     </row>
     <row r="774" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A774">
+      <c r="A774" s="1">
         <v>10</v>
       </c>
       <c r="B774" t="s">
@@ -25656,7 +25642,7 @@
       </c>
     </row>
     <row r="775" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A775" t="s">
+      <c r="A775" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="B775" t="s">
@@ -25679,7 +25665,7 @@
       </c>
     </row>
     <row r="776" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A776">
+      <c r="A776" s="1">
         <v>11</v>
       </c>
       <c r="B776" t="s">
@@ -25702,7 +25688,7 @@
       </c>
     </row>
     <row r="777" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A777" t="s">
+      <c r="A777" s="1" t="s">
         <v>1140</v>
       </c>
       <c r="B777" t="s">
@@ -25725,7 +25711,7 @@
       </c>
     </row>
     <row r="778" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A778">
+      <c r="A778" s="1">
         <v>12</v>
       </c>
       <c r="B778" t="s">
@@ -25748,7 +25734,7 @@
       </c>
     </row>
     <row r="779" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A779" t="s">
+      <c r="A779" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B779" t="s">
@@ -25771,7 +25757,7 @@
       </c>
     </row>
     <row r="780" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A780">
+      <c r="A780" s="1">
         <v>13</v>
       </c>
       <c r="B780" t="s">
@@ -25808,7 +25794,7 @@
       </c>
     </row>
     <row r="782" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A782">
+      <c r="A782" s="1">
         <v>1</v>
       </c>
       <c r="B782" t="s">
@@ -25831,7 +25817,7 @@
       </c>
     </row>
     <row r="783" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A783" t="s">
+      <c r="A783" s="1" t="s">
         <v>1069</v>
       </c>
       <c r="B783" t="s">
@@ -25854,7 +25840,7 @@
       </c>
     </row>
     <row r="784" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A784">
+      <c r="A784" s="1">
         <v>2</v>
       </c>
       <c r="B784" t="s">
@@ -25877,7 +25863,7 @@
       </c>
     </row>
     <row r="785" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A785" t="s">
+      <c r="A785" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B785" t="s">
@@ -25900,7 +25886,7 @@
       </c>
     </row>
     <row r="786" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A786">
+      <c r="A786" s="1">
         <v>3</v>
       </c>
       <c r="B786" t="s">
@@ -25923,7 +25909,7 @@
       </c>
     </row>
     <row r="787" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A787" t="s">
+      <c r="A787" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="B787" t="s">
@@ -25946,7 +25932,7 @@
       </c>
     </row>
     <row r="788" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A788">
+      <c r="A788" s="1">
         <v>4</v>
       </c>
       <c r="B788" t="s">
@@ -25969,7 +25955,7 @@
       </c>
     </row>
     <row r="789" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A789" t="s">
+      <c r="A789" s="1" t="s">
         <v>1091</v>
       </c>
       <c r="B789" t="s">
@@ -25992,7 +25978,7 @@
       </c>
     </row>
     <row r="790" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A790">
+      <c r="A790" s="1">
         <v>5</v>
       </c>
       <c r="B790" t="s">
@@ -26015,7 +26001,7 @@
       </c>
     </row>
     <row r="791" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A791" t="s">
+      <c r="A791" s="1" t="s">
         <v>1098</v>
       </c>
       <c r="B791" t="s">
@@ -26038,7 +26024,7 @@
       </c>
     </row>
     <row r="792" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A792">
+      <c r="A792" s="1">
         <v>6</v>
       </c>
       <c r="B792" t="s">
@@ -26061,7 +26047,7 @@
       </c>
     </row>
     <row r="793" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A793" t="s">
+      <c r="A793" s="1" t="s">
         <v>1105</v>
       </c>
       <c r="B793" t="s">
@@ -26084,7 +26070,7 @@
       </c>
     </row>
     <row r="794" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A794">
+      <c r="A794" s="1">
         <v>7</v>
       </c>
       <c r="B794" t="s">
@@ -26107,7 +26093,7 @@
       </c>
     </row>
     <row r="795" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A795" t="s">
+      <c r="A795" s="1" t="s">
         <v>1112</v>
       </c>
       <c r="B795" t="s">
@@ -26130,7 +26116,7 @@
       </c>
     </row>
     <row r="796" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A796">
+      <c r="A796" s="1">
         <v>8</v>
       </c>
       <c r="B796" t="s">
@@ -26153,7 +26139,7 @@
       </c>
     </row>
     <row r="797" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A797" t="s">
+      <c r="A797" s="1" t="s">
         <v>1119</v>
       </c>
       <c r="B797" t="s">
@@ -26176,7 +26162,7 @@
       </c>
     </row>
     <row r="798" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A798">
+      <c r="A798" s="1">
         <v>9</v>
       </c>
       <c r="B798" t="s">
@@ -26199,7 +26185,7 @@
       </c>
     </row>
     <row r="799" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A799" t="s">
+      <c r="A799" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="B799" t="s">
@@ -26222,7 +26208,7 @@
       </c>
     </row>
     <row r="800" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A800">
+      <c r="A800" s="1">
         <v>10</v>
       </c>
       <c r="B800" t="s">
@@ -26245,7 +26231,7 @@
       </c>
     </row>
     <row r="801" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A801" t="s">
+      <c r="A801" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="B801" t="s">
@@ -26268,7 +26254,7 @@
       </c>
     </row>
     <row r="802" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A802">
+      <c r="A802" s="1">
         <v>11</v>
       </c>
       <c r="B802" t="s">
@@ -26291,7 +26277,7 @@
       </c>
     </row>
     <row r="803" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A803" t="s">
+      <c r="A803" s="1" t="s">
         <v>1140</v>
       </c>
       <c r="B803" t="s">
@@ -26314,7 +26300,7 @@
       </c>
     </row>
     <row r="804" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A804">
+      <c r="A804" s="1">
         <v>12</v>
       </c>
       <c r="B804" t="s">
@@ -26337,7 +26323,7 @@
       </c>
     </row>
     <row r="805" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A805" t="s">
+      <c r="A805" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B805" t="s">
@@ -26360,7 +26346,7 @@
       </c>
     </row>
     <row r="806" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A806">
+      <c r="A806" s="1">
         <v>13</v>
       </c>
       <c r="B806" t="s">
@@ -26397,7 +26383,7 @@
       </c>
     </row>
     <row r="808" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A808">
+      <c r="A808" s="1">
         <v>1</v>
       </c>
       <c r="B808" t="s">
@@ -26420,7 +26406,7 @@
       </c>
     </row>
     <row r="809" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A809" t="s">
+      <c r="A809" s="1" t="s">
         <v>1069</v>
       </c>
       <c r="B809" t="s">
@@ -26443,7 +26429,7 @@
       </c>
     </row>
     <row r="810" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A810">
+      <c r="A810" s="1">
         <v>2</v>
       </c>
       <c r="B810" t="s">
@@ -26466,7 +26452,7 @@
       </c>
     </row>
     <row r="811" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A811" t="s">
+      <c r="A811" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B811" t="s">
@@ -26489,7 +26475,7 @@
       </c>
     </row>
     <row r="812" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A812">
+      <c r="A812" s="1">
         <v>3</v>
       </c>
       <c r="B812" t="s">
@@ -26512,7 +26498,7 @@
       </c>
     </row>
     <row r="813" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A813" t="s">
+      <c r="A813" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="B813" t="s">
@@ -26535,7 +26521,7 @@
       </c>
     </row>
     <row r="814" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A814">
+      <c r="A814" s="1">
         <v>4</v>
       </c>
       <c r="B814" t="s">
@@ -26558,7 +26544,7 @@
       </c>
     </row>
     <row r="815" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A815" t="s">
+      <c r="A815" s="1" t="s">
         <v>1091</v>
       </c>
       <c r="B815" t="s">
@@ -26581,7 +26567,7 @@
       </c>
     </row>
     <row r="816" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A816">
+      <c r="A816" s="1">
         <v>5</v>
       </c>
       <c r="B816" t="s">
@@ -26604,7 +26590,7 @@
       </c>
     </row>
     <row r="817" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A817" t="s">
+      <c r="A817" s="1" t="s">
         <v>1098</v>
       </c>
       <c r="B817" t="s">
@@ -26627,7 +26613,7 @@
       </c>
     </row>
     <row r="818" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A818">
+      <c r="A818" s="1">
         <v>6</v>
       </c>
       <c r="B818" t="s">
@@ -26650,7 +26636,7 @@
       </c>
     </row>
     <row r="819" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A819" t="s">
+      <c r="A819" s="1" t="s">
         <v>1105</v>
       </c>
       <c r="B819" t="s">
@@ -26673,7 +26659,7 @@
       </c>
     </row>
     <row r="820" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A820">
+      <c r="A820" s="1">
         <v>7</v>
       </c>
       <c r="B820" t="s">
@@ -26696,7 +26682,7 @@
       </c>
     </row>
     <row r="821" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A821" t="s">
+      <c r="A821" s="1" t="s">
         <v>1112</v>
       </c>
       <c r="B821" t="s">
@@ -26719,7 +26705,7 @@
       </c>
     </row>
     <row r="822" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A822">
+      <c r="A822" s="1">
         <v>8</v>
       </c>
       <c r="B822" t="s">
@@ -26742,7 +26728,7 @@
       </c>
     </row>
     <row r="823" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A823" t="s">
+      <c r="A823" s="1" t="s">
         <v>1119</v>
       </c>
       <c r="B823" t="s">
@@ -26765,7 +26751,7 @@
       </c>
     </row>
     <row r="824" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A824">
+      <c r="A824" s="1">
         <v>9</v>
       </c>
       <c r="B824" t="s">
@@ -26788,7 +26774,7 @@
       </c>
     </row>
     <row r="825" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A825" t="s">
+      <c r="A825" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="B825" t="s">
@@ -26811,7 +26797,7 @@
       </c>
     </row>
     <row r="826" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A826">
+      <c r="A826" s="1">
         <v>10</v>
       </c>
       <c r="B826" t="s">
@@ -26834,7 +26820,7 @@
       </c>
     </row>
     <row r="827" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A827" t="s">
+      <c r="A827" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="B827" t="s">
@@ -26857,7 +26843,7 @@
       </c>
     </row>
     <row r="828" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A828">
+      <c r="A828" s="1">
         <v>11</v>
       </c>
       <c r="B828" t="s">
@@ -26880,7 +26866,7 @@
       </c>
     </row>
     <row r="829" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A829" t="s">
+      <c r="A829" s="1" t="s">
         <v>1140</v>
       </c>
       <c r="B829" t="s">
@@ -26903,7 +26889,7 @@
       </c>
     </row>
     <row r="830" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A830">
+      <c r="A830" s="1">
         <v>12</v>
       </c>
       <c r="B830" t="s">
@@ -26926,7 +26912,7 @@
       </c>
     </row>
     <row r="831" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A831" t="s">
+      <c r="A831" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B831" t="s">
@@ -26949,7 +26935,7 @@
       </c>
     </row>
     <row r="832" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A832">
+      <c r="A832" s="1">
         <v>13</v>
       </c>
       <c r="B832" t="s">
@@ -26990,5 +26976,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>